<commit_message>
fix permintaan customer tyck
</commit_message>
<xml_diff>
--- a/public/doc/通用仓库-库位变更导入模板.xlsx
+++ b/public/doc/通用仓库-库位变更导入模板.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\elt-wms\public\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C022D2DD-79D7-4A58-B790-EB2890480BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE29ACD5-D0D8-4ED6-969C-38906B1692B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A3ACD4C-5513-47A8-9D88-FB190AEFB65D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>序号</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>现库位</t>
-  </si>
-  <si>
-    <t>原库位数量</t>
-  </si>
-  <si>
-    <t>现库位数量</t>
   </si>
   <si>
     <t>SMI</t>
@@ -576,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979EEEA3-24E6-4928-BCF6-F4F04C05DF85}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,12 +584,10 @@
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:9" ht="20.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -612,7 +604,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>6</v>
@@ -620,215 +612,173 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25">
+    <row r="2" spans="1:9" ht="17.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="17.25">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>5</v>
-      </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="17.25">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.25">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="2">
-        <v>5</v>
-      </c>
-      <c r="J5" s="2">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="17.25">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>10</v>
-      </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="17.25">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="17.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>5</v>
-      </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="17.25">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -838,10 +788,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="17.25">
+    </row>
+    <row r="9" spans="1:9" ht="17.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -851,10 +799,8 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="17.25">
+    </row>
+    <row r="10" spans="1:9" ht="17.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -864,10 +810,8 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.25">
+    </row>
+    <row r="11" spans="1:9" ht="17.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -877,10 +821,8 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.25">
+    </row>
+    <row r="12" spans="1:9" ht="17.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -890,10 +832,8 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="17.25">
+    </row>
+    <row r="13" spans="1:9" ht="17.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -903,10 +843,8 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="17.25">
+    </row>
+    <row r="14" spans="1:9" ht="17.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -916,10 +854,8 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.25">
+    </row>
+    <row r="15" spans="1:9" ht="17.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -929,10 +865,8 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="17.25">
+    </row>
+    <row r="16" spans="1:9" ht="17.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -942,10 +876,8 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="17.25">
+    </row>
+    <row r="17" spans="1:9" ht="17.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -955,12 +887,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:K2 I3:K5 A3:G3 E4:G4 A4:C4 A5:G5 D2:E5 A8:G17 I7:K17 K6 A6:A7">
+  <conditionalFormatting sqref="A3:G3 E4:G4 A4:C4 A5:G5 D2:E5 A8:G17 A6:A7 A2:H2 I2:I17">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -975,7 +905,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:J6">
+  <conditionalFormatting sqref="B6:H6">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>